<commit_message>
edits to clean resp var
</commit_message>
<xml_diff>
--- a/data/scrapedEgret/egret_DL.xlsx
+++ b/data/scrapedEgret/egret_DL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/egret/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdre/Documents/github/egret/data/scrapedEgret/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DAC775-9A22-074D-A842-1310830D737B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C0738C-0424-8F47-959F-2ED3B76DFD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35140" yWindow="3480" windowWidth="33400" windowHeight="16900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="18500" windowHeight="17620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -9023,7 +9023,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9054,6 +9054,8 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -9101,14 +9103,6 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -9116,6 +9110,14 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9431,7 +9433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -9995,14 +9997,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(A7))=0</formula>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(A6))=0</formula>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10013,8 +10015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="C224" sqref="C224"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12698,55 +12700,55 @@
         <v>165</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
+    <row r="51" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="24" t="s">
         <v>389</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="24" t="s">
         <v>390</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="24">
         <v>36</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F51" s="24">
         <v>1</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G51" s="24">
         <v>105</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H51" s="24">
         <v>2008</v>
       </c>
-      <c r="I51" s="10" t="s">
+      <c r="I51" s="24" t="s">
         <v>391</v>
       </c>
-      <c r="J51" s="10" t="s">
+      <c r="J51" s="24" t="s">
         <v>392</v>
       </c>
-      <c r="K51" s="10" t="s">
+      <c r="K51" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="L51" s="10"/>
-      <c r="M51" s="10"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10" t="s">
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24" t="s">
         <v>513</v>
       </c>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="10" t="s">
+      <c r="Q51" s="24"/>
+      <c r="R51" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="S51" s="10" t="s">
+      <c r="S51" s="24" t="s">
         <v>393</v>
       </c>
-      <c r="T51" s="10" t="s">
+      <c r="T51" s="24" t="s">
         <v>202</v>
       </c>
     </row>
@@ -12952,41 +12954,41 @@
         <v>594</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="25" t="s">
         <v>413</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="25" t="s">
         <v>414</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="25" t="s">
         <v>404</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="25">
         <v>2009</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" s="25" t="s">
         <v>392</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K56" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="P56" t="s">
+      <c r="P56" s="25" t="s">
         <v>513</v>
       </c>
-      <c r="R56" t="s">
+      <c r="R56" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="S56" t="s">
+      <c r="S56" s="25" t="s">
         <v>415</v>
       </c>
-      <c r="T56" t="s">
+      <c r="T56" s="25" t="s">
         <v>261</v>
       </c>
     </row>
@@ -32078,9 +32080,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS382"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE375" sqref="AE375:AE376"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AS17" sqref="AS17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33363,7 +33365,7 @@
         <v>46</v>
       </c>
       <c r="AK14">
-        <v>248</v>
+        <v>78.981999999999999</v>
       </c>
       <c r="AM14" t="s">
         <v>40</v>
@@ -33446,7 +33448,7 @@
         <v>46</v>
       </c>
       <c r="AK15">
-        <v>169.333</v>
+        <v>91.840999999999994</v>
       </c>
       <c r="AM15" t="s">
         <v>40</v>
@@ -33529,7 +33531,7 @@
         <v>46</v>
       </c>
       <c r="AK16">
-        <v>177.333</v>
+        <v>90.97</v>
       </c>
       <c r="AM16" t="s">
         <v>40</v>
@@ -33612,7 +33614,7 @@
         <v>46</v>
       </c>
       <c r="AK17">
-        <v>241.333</v>
+        <v>80.004000000000005</v>
       </c>
       <c r="AM17" t="s">
         <v>40</v>

</xml_diff>